<commit_message>
Added footer and renamed verify blade file.
1. Renamed verify page to verify-cert to avoid confusion with auth/verify blade file
2. Added footer page with app version number and author info
3. Included footer to all relevant pages
</commit_message>
<xml_diff>
--- a/downloads/Data Import Template.xlsx
+++ b/downloads/Data Import Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\verify-cert\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B670C2-C829-4DE6-8F2C-AE2A7F3F0E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC8A5F7-7FF1-4800-988E-117B5CE597DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>certificate_number</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>created_by</t>
+  </si>
+  <si>
+    <t>training_end</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" activeCellId="2" sqref="I1:I1048576 J1:J1048576 K1:K1048576"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,12 +434,13 @@
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,12 +469,15 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>